<commit_message>
Convert illusion size data into dva
</commit_message>
<xml_diff>
--- a/data/hjh_data.xlsx
+++ b/data/hjh_data.xlsx
@@ -123,418 +123,418 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6.9992857325063653</v>
+        <v>0.33925081629874615</v>
       </c>
       <c r="B2" s="0">
-        <v>15.486709909225908</v>
+        <v>0.75059656291303156</v>
       </c>
       <c r="C2" s="0">
-        <v>15.062445840513959</v>
+        <v>0.73003595300213164</v>
       </c>
       <c r="D2" s="0">
-        <v>9.9712770159707986</v>
+        <v>0.48329548166709418</v>
       </c>
       <c r="E2" s="0">
-        <v>26.515432893255024</v>
+        <v>1.2849852807769151</v>
       </c>
       <c r="F2" s="0">
-        <v>-32.879393923933975</v>
+        <v>-1.5932506216370377</v>
       </c>
       <c r="G2" s="0">
-        <v>31.184480451567168</v>
+        <v>1.5111586036666993</v>
       </c>
       <c r="H2" s="0">
-        <v>-0.21320343559642652</v>
+        <v>-0.010333952179654458</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>19.729350596345199</v>
+        <v>0.95619115610792682</v>
       </c>
       <c r="B3" s="0">
-        <v>48.577164466275377</v>
+        <v>2.3532069497846337</v>
       </c>
       <c r="C3" s="0">
-        <v>31.182337649086293</v>
+        <v>1.5110548144405425</v>
       </c>
       <c r="D3" s="0">
-        <v>-1.0595887705393352</v>
+        <v>-0.051358163344462041</v>
       </c>
       <c r="E3" s="0">
-        <v>14.638181771802039</v>
+        <v>0.70947515506068048</v>
       </c>
       <c r="F3" s="0">
-        <v>1.4838528392512842</v>
+        <v>0.071922182453363542</v>
       </c>
       <c r="G3" s="0">
-        <v>24.818376618407342</v>
+        <v>1.2027678846874374</v>
       </c>
       <c r="H3" s="0">
-        <v>-13.789653634378197</v>
+        <v>-0.66835301625825527</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>40.516147160748687</v>
+        <v>1.9630457150916616</v>
       </c>
       <c r="B4" s="0">
-        <v>22.699199077328728</v>
+        <v>1.1000930353764693</v>
       </c>
       <c r="C4" s="0">
-        <v>27.788225099390843</v>
+        <v>1.3466448731743619</v>
       </c>
       <c r="D4" s="0">
-        <v>8.6963420073540476</v>
+        <v>0.42150334937917461</v>
       </c>
       <c r="E4" s="0">
-        <v>11.668333290818509</v>
+        <v>0.5655447492585044</v>
       </c>
       <c r="F4" s="0">
-        <v>7.4235498012182859</v>
+        <v>0.35981409390636743</v>
       </c>
       <c r="G4" s="0">
-        <v>50.698484809835008</v>
+        <v>2.455846154993611</v>
       </c>
       <c r="H4" s="0">
-        <v>-41.364675298172614</v>
+        <v>-2.0041245251795918</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>13.365389565666277</v>
+        <v>0.64779168598404679</v>
       </c>
       <c r="B5" s="0">
-        <v>26.515432893255053</v>
+        <v>1.2849852807769164</v>
       </c>
       <c r="C5" s="0">
-        <v>13.789653634378141</v>
+        <v>0.6683530162582525</v>
       </c>
       <c r="D5" s="0">
-        <v>4.0294372515228645</v>
+        <v>0.19530572256204778</v>
       </c>
       <c r="E5" s="0">
-        <v>41.788939366884478</v>
+        <v>2.0246631599380729</v>
       </c>
       <c r="F5" s="0">
-        <v>15.062445840513988</v>
+        <v>0.73003595300213309</v>
       </c>
       <c r="G5" s="0">
-        <v>38.396969619669903</v>
+        <v>1.8604437006995171</v>
       </c>
       <c r="H5" s="0">
-        <v>7.8499566724111673</v>
+        <v>0.38048113569428316</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>40.091883092036767</v>
+        <v>1.9425055502821438</v>
       </c>
       <c r="B6" s="0">
-        <v>-4.4537013202347566</v>
+        <v>-0.21586950070994318</v>
       </c>
       <c r="C6" s="0">
-        <v>12.941125496954299</v>
+        <v>0.62723018885279758</v>
       </c>
       <c r="D6" s="0">
-        <v>-7.8478138699302633</v>
+        <v>-0.38037727882005812</v>
       </c>
       <c r="E6" s="0">
-        <v>34.576450198781743</v>
+        <v>1.675439869719797</v>
       </c>
       <c r="F6" s="0">
-        <v>-15.908831175456811</v>
+        <v>-0.77105313685860599</v>
       </c>
       <c r="G6" s="0">
-        <v>26.517575695736014</v>
+        <v>1.2850890899941976</v>
       </c>
       <c r="H6" s="0">
-        <v>-4.8801081914276381</v>
+        <v>-0.23653708292768558</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>23.123463146040621</v>
+        <v>1.1206493560114417</v>
       </c>
       <c r="B7" s="0">
-        <v>6.1507575950824958</v>
+        <v>0.29812400418901785</v>
       </c>
       <c r="C7" s="0">
-        <v>41.788939366884478</v>
+        <v>2.0246631599380729</v>
       </c>
       <c r="D7" s="0">
-        <v>-3.1809091140989665</v>
+        <v>-0.15417802061515548</v>
       </c>
       <c r="E7" s="0">
-        <v>5.7286363288515361</v>
+        <v>0.27766433929563522</v>
       </c>
       <c r="F7" s="0">
-        <v>-0.63746750430837551</v>
+        <v>-0.030897992426927895</v>
       </c>
       <c r="G7" s="0">
-        <v>39.667619023324846</v>
+        <v>1.9219648859768377</v>
       </c>
       <c r="H7" s="0">
-        <v>8.696342007354076</v>
+        <v>0.42150334937917588</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>35.849242404917504</v>
+        <v>1.7370772983798759</v>
       </c>
       <c r="B8" s="0">
-        <v>12.941125496954271</v>
+        <v>0.62723018885279624</v>
       </c>
       <c r="C8" s="0">
-        <v>34.152186130069765</v>
+        <v>1.6548931910713423</v>
       </c>
       <c r="D8" s="0">
-        <v>6.5750216637944163</v>
+        <v>0.31868745129398518</v>
       </c>
       <c r="E8" s="0">
-        <v>23.54772721475257</v>
+        <v>1.1412053881140662</v>
       </c>
       <c r="F8" s="0">
-        <v>-5.3043722601396155</v>
+        <v>-0.25710074422938334</v>
       </c>
       <c r="G8" s="0">
-        <v>34.152186130069794</v>
+        <v>1.6548931910713434</v>
       </c>
       <c r="H8" s="0">
-        <v>9.9712770159708271</v>
+        <v>0.48329548166709557</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-2.7566450453871028</v>
+        <v>-0.13361410741152846</v>
       </c>
       <c r="B9" s="0">
-        <v>10.393398282201787</v>
+        <v>0.50375414512813355</v>
       </c>
       <c r="C9" s="0">
-        <v>5.3043722601395871</v>
+        <v>0.25710074422938201</v>
       </c>
       <c r="D9" s="0">
-        <v>-10.395541084682748</v>
+        <v>-0.50385799855097857</v>
       </c>
       <c r="E9" s="0">
-        <v>27.788225099390871</v>
+        <v>1.346644873174363</v>
       </c>
       <c r="F9" s="0">
-        <v>-26.091168824543189</v>
+        <v>-1.2644314147142786</v>
       </c>
       <c r="G9" s="0">
-        <v>15.910973977937829</v>
+        <v>0.77115697950070472</v>
       </c>
       <c r="H9" s="0">
-        <v>-27.7882250993909</v>
+        <v>-1.3466448731743643</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>37.122034611053266</v>
+        <v>1.7987107054527727</v>
       </c>
       <c r="B10" s="0">
-        <v>8.2742207411230879</v>
+        <v>0.40104422210902801</v>
       </c>
       <c r="C10" s="0">
-        <v>17.18376618407359</v>
+        <v>0.83283701640217245</v>
       </c>
       <c r="D10" s="0">
-        <v>12.092597359530515</v>
+        <v>0.58610671519561719</v>
       </c>
       <c r="E10" s="0">
-        <v>26.091168824543189</v>
+        <v>1.2644314147142786</v>
       </c>
       <c r="F10" s="0">
-        <v>-34.576450198781743</v>
+        <v>-1.675439869719797</v>
       </c>
       <c r="G10" s="0">
-        <v>19.729350596345199</v>
+        <v>0.95619115610792682</v>
       </c>
       <c r="H10" s="0">
-        <v>7.4235498012182859</v>
+        <v>0.35981409390636743</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>1.9102597104441656</v>
+        <v>0.092590044214865566</v>
       </c>
       <c r="B11" s="0">
-        <v>31.182337649086321</v>
+        <v>1.5110548144405438</v>
       </c>
       <c r="C11" s="0">
-        <v>29.061017305526661</v>
+        <v>1.4083013459858935</v>
       </c>
       <c r="D11" s="0">
-        <v>-12.514718625761446</v>
+        <v>-0.60656468034737943</v>
       </c>
       <c r="E11" s="0">
-        <v>9.9712770159707986</v>
+        <v>0.48329548166709418</v>
       </c>
       <c r="F11" s="0">
-        <v>11.241926419625685</v>
+        <v>0.54487878558359215</v>
       </c>
       <c r="G11" s="0">
-        <v>51.547012947258878</v>
+        <v>2.4968974583591708</v>
       </c>
       <c r="H11" s="0">
-        <v>8.696342007354076</v>
+        <v>0.42150334937917588</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>27.363961030678922</v>
+        <v>1.3260920152884488</v>
       </c>
       <c r="B12" s="0">
-        <v>12.092597359530487</v>
+        <v>0.58610671519561564</v>
       </c>
       <c r="C12" s="0">
-        <v>39.667619023324875</v>
+        <v>1.9219648859768388</v>
       </c>
       <c r="D12" s="0">
-        <v>7.8478138699302633</v>
+        <v>0.38037727882005812</v>
       </c>
       <c r="E12" s="0">
-        <v>7.4256926036992184</v>
+        <v>0.35991795126220039</v>
       </c>
       <c r="F12" s="0">
-        <v>-1.4859956417322167</v>
+        <v>-0.072026043742483573</v>
       </c>
       <c r="G12" s="0">
-        <v>40.516147160748716</v>
+        <v>1.9630457150916636</v>
       </c>
       <c r="H12" s="0">
-        <v>-17.181623381592658</v>
+        <v>-0.83273317688955373</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>-3.1809091140989949</v>
+        <v>-0.15417802061515684</v>
       </c>
       <c r="B13" s="0">
-        <v>16.333095244168817</v>
+        <v>0.79161335584711523</v>
       </c>
       <c r="C13" s="0">
-        <v>17.18376618407359</v>
+        <v>0.83283701640217245</v>
       </c>
       <c r="D13" s="0">
-        <v>-9.1227488785469575</v>
+        <v>-0.44217007970067068</v>
       </c>
       <c r="E13" s="0">
-        <v>33.303657992645896</v>
+        <v>1.6137985617578119</v>
       </c>
       <c r="F13" s="0">
-        <v>13.365389565666248</v>
+        <v>0.64779168598404546</v>
       </c>
       <c r="G13" s="0">
-        <v>25.244783489600252</v>
+        <v>1.2234265254958585</v>
       </c>
       <c r="H13" s="0">
-        <v>-10.817662350913736</v>
+        <v>-0.52431653288708802</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>35.000714267493635</v>
+        <v>1.6959861173342601</v>
       </c>
       <c r="B14" s="0">
-        <v>10.395541084682748</v>
+        <v>0.50385799855097857</v>
       </c>
       <c r="C14" s="0">
-        <v>8.2742207411231163</v>
+        <v>0.4010442221090294</v>
       </c>
       <c r="D14" s="0">
-        <v>-6.5750216637944163</v>
+        <v>-0.31868745129398518</v>
       </c>
       <c r="E14" s="0">
-        <v>35.849242404917504</v>
+        <v>1.7370772983798759</v>
       </c>
       <c r="F14" s="0">
-        <v>-32.030865786510162</v>
+        <v>-1.5521535168330414</v>
       </c>
       <c r="G14" s="0">
-        <v>24.396255352176382</v>
+        <v>1.182316565580303</v>
       </c>
       <c r="H14" s="0">
-        <v>-1.0617315730203245</v>
+        <v>-0.051462024713859106</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>7.8499566724111105</v>
+        <v>0.38048113569428038</v>
       </c>
       <c r="B15" s="0">
-        <v>14.636038969321078</v>
+        <v>0.7093713095296702</v>
       </c>
       <c r="C15" s="0">
-        <v>12.938982694473339</v>
+        <v>0.62712633984417754</v>
       </c>
       <c r="D15" s="0">
-        <v>-38.819090885901034</v>
+        <v>-1.8808820799272301</v>
       </c>
       <c r="E15" s="0">
-        <v>12.092597359530458</v>
+        <v>0.5861067151956143</v>
       </c>
       <c r="F15" s="0">
-        <v>-2.3345237791560578</v>
+        <v>-0.113154020833087</v>
       </c>
       <c r="G15" s="0">
-        <v>33.727922061357873</v>
+        <v>1.6343460866600741</v>
       </c>
       <c r="H15" s="0">
-        <v>2.3323809766751253</v>
+        <v>0.11305015978478901</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>18.878679656440369</v>
+        <v>0.9149702030785184</v>
       </c>
       <c r="B16" s="0">
-        <v>20.577878733769097</v>
+        <v>0.99730728924314882</v>
       </c>
       <c r="C16" s="0">
-        <v>18.030151519016471</v>
+        <v>0.87385214007582646</v>
       </c>
       <c r="D16" s="0">
-        <v>13.363246763185316</v>
+        <v>0.64768783780472416</v>
       </c>
       <c r="E16" s="0">
-        <v>13.36538956566622</v>
+        <v>0.64779168598404413</v>
       </c>
       <c r="F16" s="0">
-        <v>-7.4256926036992184</v>
+        <v>-0.35991795126220039</v>
       </c>
       <c r="G16" s="0">
-        <v>43.061731573020325</v>
+        <v>2.0862759199687408</v>
       </c>
       <c r="H16" s="0">
-        <v>-6.9992857325063653</v>
+        <v>-0.33925081629874615</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>-9.9691342134898946</v>
+        <v>-0.48319162760215162</v>
       </c>
       <c r="B17" s="0">
-        <v>12.514718625761446</v>
+        <v>0.60656468034737943</v>
       </c>
       <c r="C17" s="0">
-        <v>9.1227488785469575</v>
+        <v>0.44217007970067068</v>
       </c>
       <c r="D17" s="0">
-        <v>-5.3043722601395871</v>
+        <v>-0.25710074422938201</v>
       </c>
       <c r="E17" s="0">
-        <v>24.818376618407342</v>
+        <v>1.2027678846874374</v>
       </c>
       <c r="F17" s="0">
-        <v>-8.2720779386421555</v>
+        <v>-0.40094036574315933</v>
       </c>
       <c r="G17" s="0">
-        <v>14.638181771802039</v>
+        <v>0.70947515506068048</v>
       </c>
       <c r="H17" s="0">
-        <v>7.4256926036992184</v>
+        <v>0.35991795126220039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>